<commit_message>
Added most recent two games
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -280,10 +280,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -310,16 +310,22 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Z$2:$Z$10</c:f>
+              <c:f>Sheet1!$Z$2:$Z$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>200</c:v>
                 </c:pt>
@@ -346,6 +352,12 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>157.44444444444446</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>154.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>151.72727272727272</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -685,7 +697,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -1998,16 +2010,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2072,8 +2084,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AA10" totalsRowShown="0">
-  <autoFilter ref="A1:AA10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AA12" totalsRowShown="0">
+  <autoFilter ref="A1:AA12"/>
   <tableColumns count="27">
     <tableColumn id="1" name="Game #">
       <calculatedColumnFormula>A1+1</calculatedColumnFormula>
@@ -2591,7 +2603,7 @@
       </c>
       <c r="AC2">
         <f>SUM(Table1[Strikes])</f>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="AE2">
         <v>0</v>
@@ -2687,12 +2699,12 @@
       </c>
       <c r="AF3">
         <f>COUNTIF(Table1[Strikes],AE3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A10" si="1">A3+1</f>
+        <f t="shared" ref="A4:A11" si="1">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1">
@@ -2765,7 +2777,7 @@
       </c>
       <c r="AC4">
         <f>AVERAGE(Table1[Strikes])</f>
-        <v>3.5555555555555554</v>
+        <v>3.0909090909090908</v>
       </c>
       <c r="AE4">
         <f t="shared" ref="AE4:AE14" si="2">AE3+1</f>
@@ -3296,6 +3308,84 @@
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>A10+1</f>
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>42975</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>8</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>7</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>9</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>8</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>8</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>7</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>4</v>
+      </c>
+      <c r="S11">
+        <v>6</v>
+      </c>
+      <c r="T11">
+        <v>10</v>
+      </c>
+      <c r="V11">
+        <v>6</v>
+      </c>
+      <c r="W11">
+        <v>3</v>
+      </c>
+      <c r="Y11">
+        <v>132</v>
+      </c>
+      <c r="Z11">
+        <f>AVERAGE($Y$2:Y11)</f>
+        <v>154.9</v>
+      </c>
+      <c r="AA11">
+        <f>COUNTIF(D11:X11,10)</f>
+        <v>1</v>
+      </c>
       <c r="AE11">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -3306,6 +3396,84 @@
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>A11+1</f>
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>42975</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>8</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>7</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+      <c r="J12">
+        <v>7</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+      <c r="L12">
+        <v>10</v>
+      </c>
+      <c r="N12">
+        <v>8</v>
+      </c>
+      <c r="O12">
+        <v>2</v>
+      </c>
+      <c r="P12">
+        <v>3</v>
+      </c>
+      <c r="Q12">
+        <v>6</v>
+      </c>
+      <c r="R12">
+        <v>6</v>
+      </c>
+      <c r="S12">
+        <v>3</v>
+      </c>
+      <c r="T12">
+        <v>7</v>
+      </c>
+      <c r="U12">
+        <v>1</v>
+      </c>
+      <c r="V12">
+        <v>5</v>
+      </c>
+      <c r="W12">
+        <v>1</v>
+      </c>
+      <c r="Y12">
+        <v>120</v>
+      </c>
+      <c r="Z12">
+        <f>AVERAGE($Y$2:Y12)</f>
+        <v>151.72727272727272</v>
+      </c>
+      <c r="AA12">
+        <f>COUNTIF(E12:X12,10)</f>
+        <v>1</v>
+      </c>
       <c r="AE12">
         <f t="shared" si="2"/>
         <v>10</v>

</xml_diff>

<commit_message>
Added games from the 2/9/17 and 3/9/17
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -116,7 +116,7 @@
     <t>10.3</t>
   </si>
   <si>
-    <t>Column2</t>
+    <t>Best Game</t>
   </si>
 </sst>
 </file>
@@ -159,7 +159,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
@@ -280,10 +283,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>Sheet1!$A$2:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -316,16 +319,34 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Z$2:$Z$12</c:f>
+              <c:f>Sheet1!$Z$2:$Z$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>200</c:v>
                 </c:pt>
@@ -358,6 +379,24 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>151.72727272727272</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>150.25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>150.76923076923077</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>149.42857142857142</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>147.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>144.375</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>143.35294117647058</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -585,7 +624,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-AU"/>
-              <a:t>Gmaes with n strikes</a:t>
+              <a:t>Games with n strikes</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -629,6 +668,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>#strikes</c:v>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -641,7 +683,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$AE$2:$AE$14</c:f>
+              <c:f>Sheet1!$AF$1:$AR$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -689,24 +731,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AF$2:$AF$14</c:f>
+              <c:f>Sheet1!$AF$2:$AR$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -2010,16 +2052,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2046,16 +2088,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2084,13 +2126,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AA12" totalsRowShown="0">
-  <autoFilter ref="A1:AA12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AA18" totalsRowShown="0">
+  <autoFilter ref="A1:AA18"/>
   <tableColumns count="27">
     <tableColumn id="1" name="Game #">
       <calculatedColumnFormula>A1+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Date" dataDxfId="0"/>
+    <tableColumn id="2" name="Date" dataDxfId="1"/>
     <tableColumn id="3" name="Lane"/>
     <tableColumn id="4" name="1.1"/>
     <tableColumn id="5" name="1.2"/>
@@ -2114,7 +2156,7 @@
     <tableColumn id="23" name="10.2"/>
     <tableColumn id="24" name="10.3"/>
     <tableColumn id="25" name="Total"/>
-    <tableColumn id="26" name="Average">
+    <tableColumn id="26" name="Average" dataDxfId="0">
       <calculatedColumnFormula>AVERAGE($Y$2:Y2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="30" name="Strikes">
@@ -2422,7 +2464,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF14"/>
+  <dimension ref="A1:AR18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2437,7 +2479,7 @@
     <col min="28" max="28" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -2519,14 +2561,69 @@
       <c r="AA1" t="s">
         <v>4</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AB1" t="s">
         <v>30</v>
+      </c>
+      <c r="AC1">
+        <f>MAX(Table1[Total])</f>
+        <v>259</v>
       </c>
       <c r="AE1" t="s">
         <v>4</v>
       </c>
+      <c r="AF1">
+        <v>0</v>
+      </c>
+      <c r="AG1">
+        <f>AF1+1</f>
+        <v>1</v>
+      </c>
+      <c r="AH1">
+        <f>AG1+1</f>
+        <v>2</v>
+      </c>
+      <c r="AI1">
+        <f>AH1+1</f>
+        <v>3</v>
+      </c>
+      <c r="AJ1">
+        <f>AI1+1</f>
+        <v>4</v>
+      </c>
+      <c r="AK1">
+        <f>AJ1+1</f>
+        <v>5</v>
+      </c>
+      <c r="AL1">
+        <f>AK1+1</f>
+        <v>6</v>
+      </c>
+      <c r="AM1">
+        <f>AL1+1</f>
+        <v>7</v>
+      </c>
+      <c r="AN1">
+        <f>AM1+1</f>
+        <v>8</v>
+      </c>
+      <c r="AO1">
+        <f>AN1+1</f>
+        <v>9</v>
+      </c>
+      <c r="AP1">
+        <f>AO1+1</f>
+        <v>10</v>
+      </c>
+      <c r="AQ1">
+        <f>AP1+1</f>
+        <v>11</v>
+      </c>
+      <c r="AR1">
+        <f>AQ1+1</f>
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2603,17 +2700,62 @@
       </c>
       <c r="AC2">
         <f>SUM(Table1[Strikes])</f>
-        <v>34</v>
-      </c>
-      <c r="AE2">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="AF2">
-        <f>COUNTIF(Table1[Strikes],AE2)</f>
-        <v>1</v>
+        <f>COUNTIF(Table1[Strikes],AF1)</f>
+        <v>2</v>
+      </c>
+      <c r="AG2">
+        <f>COUNTIF(Table1[Strikes],AG1)</f>
+        <v>4</v>
+      </c>
+      <c r="AH2">
+        <f>COUNTIF(Table1[Strikes],AH1)</f>
+        <v>3</v>
+      </c>
+      <c r="AI2">
+        <f>COUNTIF(Table1[Strikes],AI1)</f>
+        <v>3</v>
+      </c>
+      <c r="AJ2">
+        <f>COUNTIF(Table1[Strikes],AJ1)</f>
+        <v>2</v>
+      </c>
+      <c r="AK2">
+        <f>COUNTIF(Table1[Strikes],AK1)</f>
+        <v>1</v>
+      </c>
+      <c r="AL2">
+        <f>COUNTIF(Table1[Strikes],AL1)</f>
+        <v>1</v>
+      </c>
+      <c r="AM2">
+        <f>COUNTIF(Table1[Strikes],AM1)</f>
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <f>COUNTIF(Table1[Strikes],AN1)</f>
+        <v>1</v>
+      </c>
+      <c r="AO2">
+        <f>COUNTIF(Table1[Strikes],AO1)</f>
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <f>COUNTIF(Table1[Strikes],AP1)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <f>COUNTIF(Table1[Strikes],AQ1)</f>
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <f>COUNTIF(Table1[Strikes],AR1)</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -2693,18 +2835,10 @@
         <f>MAX(Table1[Strikes])</f>
         <v>8</v>
       </c>
-      <c r="AE3">
-        <f>AE2+1</f>
-        <v>1</v>
-      </c>
-      <c r="AF3">
-        <f>COUNTIF(Table1[Strikes],AE3)</f>
-        <v>3</v>
-      </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A11" si="1">A3+1</f>
+        <f t="shared" ref="A4:A10" si="1">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1">
@@ -2777,18 +2911,10 @@
       </c>
       <c r="AC4">
         <f>AVERAGE(Table1[Strikes])</f>
-        <v>3.0909090909090908</v>
-      </c>
-      <c r="AE4">
-        <f t="shared" ref="AE4:AE14" si="2">AE3+1</f>
-        <v>2</v>
-      </c>
-      <c r="AF4">
-        <f>COUNTIF(Table1[Strikes],AE4)</f>
-        <v>1</v>
+        <v>2.7058823529411766</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -2870,16 +2996,8 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="AE5">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="AF5">
-        <f>COUNTIF(Table1[Strikes],AE5)</f>
-        <v>2</v>
-      </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -2943,16 +3061,8 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="AE6">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="AF6">
-        <f>COUNTIF(Table1[Strikes],AE6)</f>
-        <v>1</v>
-      </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -3031,16 +3141,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AE7">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="AF7">
-        <f>COUNTIF(Table1[Strikes],AE7)</f>
-        <v>1</v>
-      </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -3113,19 +3215,11 @@
         <v>172.28571428571428</v>
       </c>
       <c r="AA8">
-        <f t="shared" ref="AA8:AA10" si="3">COUNTIF(D8:X8,10)</f>
+        <f t="shared" ref="AA8:AA10" si="2">COUNTIF(D8:X8,10)</f>
         <v>5</v>
       </c>
-      <c r="AE8">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="AF8">
-        <f>COUNTIF(Table1[Strikes],AE8)</f>
-        <v>1</v>
-      </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -3204,19 +3298,11 @@
         <v>166.375</v>
       </c>
       <c r="AA9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="AE9">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="AF9">
-        <f>COUNTIF(Table1[Strikes],AE9)</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -3295,19 +3381,11 @@
         <v>157.44444444444446</v>
       </c>
       <c r="AA10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AE10">
         <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="AF10">
-        <f>COUNTIF(Table1[Strikes],AE10)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>A10+1</f>
         <v>10</v>
@@ -3386,16 +3464,8 @@
         <f>COUNTIF(D11:X11,10)</f>
         <v>1</v>
       </c>
-      <c r="AE11">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="AF11">
-        <f>COUNTIF(Table1[Strikes],AE11)</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>A11+1</f>
         <v>11</v>
@@ -3474,33 +3544,473 @@
         <f>COUNTIF(E12:X12,10)</f>
         <v>1</v>
       </c>
-      <c r="AE12">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="AF12">
-        <f>COUNTIF(Table1[Strikes],AE12)</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="AE13">
-        <f t="shared" si="2"/>
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>A12+1</f>
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>42980</v>
+      </c>
+      <c r="C13">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>9</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>8</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <v>6</v>
+      </c>
+      <c r="M13">
+        <v>3</v>
+      </c>
+      <c r="N13">
+        <v>7</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
+      </c>
+      <c r="P13">
+        <v>10</v>
+      </c>
+      <c r="R13">
+        <v>9</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>10</v>
+      </c>
+      <c r="V13">
+        <v>9</v>
+      </c>
+      <c r="W13">
+        <v>1</v>
+      </c>
+      <c r="X13">
+        <v>6</v>
+      </c>
+      <c r="Y13">
+        <v>134</v>
+      </c>
+      <c r="Z13">
+        <f>AVERAGE($Y$2:Y13)</f>
+        <v>150.25</v>
+      </c>
+      <c r="AA13">
+        <f>COUNTIF(D13:X13,10)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>A13+1</f>
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>42980</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="F14">
+        <v>7</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="J14">
+        <v>10</v>
+      </c>
+      <c r="L14">
+        <v>9</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>7</v>
+      </c>
+      <c r="O14">
+        <v>2</v>
+      </c>
+      <c r="P14">
+        <v>8</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>9</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>10</v>
+      </c>
+      <c r="V14">
+        <v>6</v>
+      </c>
+      <c r="W14">
+        <v>2</v>
+      </c>
+      <c r="Y14">
+        <v>157</v>
+      </c>
+      <c r="Z14">
+        <f>AVERAGE($Y$2:Y14)</f>
+        <v>150.76923076923077</v>
+      </c>
+      <c r="AA14">
+        <f>COUNTIF(D14:X14,10)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>A14+1</f>
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>42980</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>9</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>7</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="H15">
+        <v>8</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>7</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>5</v>
+      </c>
+      <c r="M15">
+        <v>4</v>
+      </c>
+      <c r="N15">
+        <v>10</v>
+      </c>
+      <c r="P15">
+        <v>10</v>
+      </c>
+      <c r="R15">
+        <v>8</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>8</v>
+      </c>
+      <c r="U15">
+        <v>2</v>
+      </c>
+      <c r="V15">
+        <v>6</v>
+      </c>
+      <c r="W15">
+        <v>3</v>
+      </c>
+      <c r="Y15">
+        <v>132</v>
+      </c>
+      <c r="Z15">
+        <f>AVERAGE($Y$2:Y15)</f>
+        <v>149.42857142857142</v>
+      </c>
+      <c r="AA15">
+        <f>COUNTIF(D15:X15,10)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f>A15+1</f>
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>42981</v>
+      </c>
+      <c r="C16">
         <v>11</v>
       </c>
-      <c r="AF13">
-        <f>COUNTIF(Table1[Strikes],AE13)</f>
-        <v>0</v>
+      <c r="D16">
+        <v>9</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>10</v>
+      </c>
+      <c r="H16">
+        <v>9</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>10</v>
+      </c>
+      <c r="L16">
+        <v>6</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>7</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>8</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>9</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>10</v>
+      </c>
+      <c r="V16">
+        <v>8</v>
+      </c>
+      <c r="W16">
+        <v>2</v>
+      </c>
+      <c r="X16">
+        <v>7</v>
+      </c>
+      <c r="Y16">
+        <v>123</v>
+      </c>
+      <c r="Z16">
+        <f>AVERAGE($Y$2:Y16)</f>
+        <v>147.66666666666666</v>
+      </c>
+      <c r="AA16">
+        <f>COUNTIF(D16:X16,10)</f>
+        <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="AE14">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="AF14">
-        <f>COUNTIF(Table1[Strikes],AE14)</f>
-        <v>0</v>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f>A16+1</f>
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>42981</v>
+      </c>
+      <c r="C17">
+        <v>11</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>6</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>7</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>8</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>3</v>
+      </c>
+      <c r="O17">
+        <v>6</v>
+      </c>
+      <c r="P17">
+        <v>8</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="R17">
+        <v>8</v>
+      </c>
+      <c r="S17">
+        <v>2</v>
+      </c>
+      <c r="T17">
+        <v>7</v>
+      </c>
+      <c r="U17">
+        <v>2</v>
+      </c>
+      <c r="V17">
+        <v>6</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>95</v>
+      </c>
+      <c r="Z17">
+        <f>AVERAGE($Y$2:Y17)</f>
+        <v>144.375</v>
+      </c>
+      <c r="AA17">
+        <f>COUNTIF(D17:X17,10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f>A17+1</f>
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>42981</v>
+      </c>
+      <c r="C18">
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>8</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <v>10</v>
+      </c>
+      <c r="L18">
+        <v>3</v>
+      </c>
+      <c r="M18">
+        <v>5</v>
+      </c>
+      <c r="N18">
+        <v>9</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>8</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18">
+        <v>9</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
+      <c r="U18">
+        <v>9</v>
+      </c>
+      <c r="V18">
+        <v>6</v>
+      </c>
+      <c r="W18">
+        <v>3</v>
+      </c>
+      <c r="Y18">
+        <v>127</v>
+      </c>
+      <c r="Z18">
+        <f>AVERAGE($Y$2:Y18)</f>
+        <v>143.35294117647058</v>
+      </c>
+      <c r="AA18">
+        <f>COUNTIF(D18:X18,10)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated games from 9/9/2017
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -123,6 +123,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -152,9 +155,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -164,7 +168,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -283,10 +287,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$18</c:f>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -337,16 +341,25 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Z$2:$Z$18</c:f>
+              <c:f>Sheet1!$Z$2:$Z$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>200</c:v>
                 </c:pt>
@@ -397,6 +410,15 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>143.35294117647058</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>146.72222222222223</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>146.73684210526315</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>146.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -745,13 +767,13 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -2126,8 +2148,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AA18" totalsRowShown="0">
-  <autoFilter ref="A1:AA18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AA21" totalsRowShown="0">
+  <autoFilter ref="A1:AA21"/>
   <tableColumns count="27">
     <tableColumn id="1" name="Game #">
       <calculatedColumnFormula>A1+1</calculatedColumnFormula>
@@ -2464,14 +2486,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR18"/>
+  <dimension ref="A1:AR21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="21" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="22" max="24" width="6.85546875" bestFit="1" customWidth="1"/>
@@ -2575,51 +2597,51 @@
         <v>0</v>
       </c>
       <c r="AG1">
-        <f>AF1+1</f>
+        <f t="shared" ref="AG1:AR1" si="0">AF1+1</f>
         <v>1</v>
       </c>
       <c r="AH1">
-        <f>AG1+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AI1">
-        <f>AH1+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="AJ1">
-        <f>AI1+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="AK1">
-        <f>AJ1+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="AL1">
-        <f>AK1+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="AM1">
-        <f>AL1+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="AN1">
-        <f>AM1+1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="AO1">
-        <f>AN1+1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="AP1">
-        <f>AO1+1</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="AQ1">
-        <f>AP1+1</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="AR1">
-        <f>AQ1+1</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
@@ -2692,7 +2714,7 @@
         <v>200</v>
       </c>
       <c r="AA2">
-        <f t="shared" ref="AA2:AA7" si="0">COUNTIF(D2:X2,10)</f>
+        <f t="shared" ref="AA2:AA7" si="1">COUNTIF(D2:X2,10)</f>
         <v>6</v>
       </c>
       <c r="AB2" t="s">
@@ -2700,7 +2722,7 @@
       </c>
       <c r="AC2">
         <f>SUM(Table1[Strikes])</f>
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="AF2">
         <f>COUNTIF(Table1[Strikes],AF1)</f>
@@ -2716,7 +2738,7 @@
       </c>
       <c r="AI2">
         <f>COUNTIF(Table1[Strikes],AI1)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AJ2">
         <f>COUNTIF(Table1[Strikes],AJ1)</f>
@@ -2724,7 +2746,7 @@
       </c>
       <c r="AK2">
         <f>COUNTIF(Table1[Strikes],AK1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL2">
         <f>COUNTIF(Table1[Strikes],AL1)</f>
@@ -2825,7 +2847,7 @@
         <v>183</v>
       </c>
       <c r="AA3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="AB3" t="s">
@@ -2838,7 +2860,7 @@
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A10" si="1">A3+1</f>
+        <f t="shared" ref="A4:A10" si="2">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1">
@@ -2903,7 +2925,7 @@
         <v>170.33333333333334</v>
       </c>
       <c r="AA4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="AB4" t="s">
@@ -2911,12 +2933,12 @@
       </c>
       <c r="AC4">
         <f>AVERAGE(Table1[Strikes])</f>
-        <v>2.7058823529411766</v>
+        <v>2.85</v>
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="B5" s="1">
@@ -2993,13 +3015,13 @@
         <v>160.75</v>
       </c>
       <c r="AA5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="B6" s="1">
@@ -3058,13 +3080,13 @@
         <v>180.4</v>
       </c>
       <c r="AA6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="B7" s="1">
@@ -3138,13 +3160,13 @@
         <v>172.5</v>
       </c>
       <c r="AA7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="B8" s="1">
@@ -3215,13 +3237,13 @@
         <v>172.28571428571428</v>
       </c>
       <c r="AA8">
-        <f t="shared" ref="AA8:AA10" si="2">COUNTIF(D8:X8,10)</f>
+        <f t="shared" ref="AA8:AA10" si="3">COUNTIF(D8:X8,10)</f>
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="B9" s="1">
@@ -3298,13 +3320,13 @@
         <v>166.375</v>
       </c>
       <c r="AA9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="B10" s="1">
@@ -3381,13 +3403,13 @@
         <v>157.44444444444446</v>
       </c>
       <c r="AA10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>A10+1</f>
+        <f t="shared" ref="A11:A19" si="4">A10+1</f>
         <v>10</v>
       </c>
       <c r="B11" s="1">
@@ -3467,7 +3489,7 @@
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>A11+1</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="B12" s="1">
@@ -3547,7 +3569,7 @@
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>A12+1</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="B13" s="1">
@@ -3621,13 +3643,13 @@
         <v>150.25</v>
       </c>
       <c r="AA13">
-        <f>COUNTIF(D13:X13,10)</f>
+        <f t="shared" ref="AA13:AA18" si="5">COUNTIF(D13:X13,10)</f>
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f>A13+1</f>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="B14" s="1">
@@ -3692,13 +3714,13 @@
         <v>150.76923076923077</v>
       </c>
       <c r="AA14">
-        <f>COUNTIF(D14:X14,10)</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f>A14+1</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="B15" s="1">
@@ -3769,13 +3791,13 @@
         <v>149.42857142857142</v>
       </c>
       <c r="AA15">
-        <f>COUNTIF(D15:X15,10)</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>A15+1</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="B16" s="1">
@@ -3846,13 +3868,13 @@
         <v>147.66666666666666</v>
       </c>
       <c r="AA16">
-        <f>COUNTIF(D16:X16,10)</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f>A16+1</f>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="B17" s="1">
@@ -3929,13 +3951,13 @@
         <v>144.375</v>
       </c>
       <c r="AA17">
-        <f>COUNTIF(D17:X17,10)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>A17+1</f>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="B18" s="1">
@@ -4009,8 +4031,236 @@
         <v>143.35294117647058</v>
       </c>
       <c r="AA18">
-        <f>COUNTIF(D18:X18,10)</f>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f>A18+1</f>
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>42987</v>
+      </c>
+      <c r="C19">
+        <v>11</v>
+      </c>
+      <c r="D19">
+        <v>7</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>10</v>
+      </c>
+      <c r="H19">
+        <v>10</v>
+      </c>
+      <c r="J19">
+        <v>10</v>
+      </c>
+      <c r="L19">
+        <v>7</v>
+      </c>
+      <c r="M19">
+        <v>3</v>
+      </c>
+      <c r="N19">
+        <v>2</v>
+      </c>
+      <c r="O19">
+        <v>8</v>
+      </c>
+      <c r="P19">
+        <v>10</v>
+      </c>
+      <c r="R19">
+        <v>7</v>
+      </c>
+      <c r="S19">
+        <v>3</v>
+      </c>
+      <c r="T19">
+        <v>10</v>
+      </c>
+      <c r="V19">
+        <v>9</v>
+      </c>
+      <c r="W19">
+        <v>1</v>
+      </c>
+      <c r="X19">
+        <v>5</v>
+      </c>
+      <c r="Y19">
+        <v>204</v>
+      </c>
+      <c r="Z19">
+        <f>AVERAGE($Y$2:Y19)</f>
+        <v>146.72222222222223</v>
+      </c>
+      <c r="AA19">
+        <f>COUNTIF(D19:X19,10)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f>A19+1</f>
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>42987</v>
+      </c>
+      <c r="C20">
+        <v>11</v>
+      </c>
+      <c r="D20">
+        <v>7</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>10</v>
+      </c>
+      <c r="H20">
+        <v>10</v>
+      </c>
+      <c r="J20">
+        <v>9</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>10</v>
+      </c>
+      <c r="N20">
+        <v>9</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>8</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>8</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20">
+        <v>9</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>7</v>
+      </c>
+      <c r="W20">
+        <v>3</v>
+      </c>
+      <c r="X20">
+        <v>5</v>
+      </c>
+      <c r="Y20">
+        <v>147</v>
+      </c>
+      <c r="Z20">
+        <f>AVERAGE($Y$2:Y20)</f>
+        <v>146.73684210526315</v>
+      </c>
+      <c r="AA20">
+        <f>COUNTIF(D20:X20,10)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f>A20+1</f>
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>42987</v>
+      </c>
+      <c r="C21">
+        <v>11</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>6</v>
+      </c>
+      <c r="H21">
+        <v>9</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>10</v>
+      </c>
+      <c r="L21">
+        <v>7</v>
+      </c>
+      <c r="M21">
+        <v>3</v>
+      </c>
+      <c r="N21">
+        <v>7</v>
+      </c>
+      <c r="O21">
+        <v>3</v>
+      </c>
+      <c r="P21">
+        <v>10</v>
+      </c>
+      <c r="R21">
+        <v>8</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <v>5</v>
+      </c>
+      <c r="U21">
+        <v>4</v>
+      </c>
+      <c r="V21">
+        <v>10</v>
+      </c>
+      <c r="W21">
+        <v>6</v>
+      </c>
+      <c r="X21">
+        <v>3</v>
+      </c>
+      <c r="Y21">
+        <v>150</v>
+      </c>
+      <c r="Z21">
+        <f>AVERAGE($Y$2:Y21)</f>
+        <v>146.9</v>
+      </c>
+      <c r="AA21">
+        <f>COUNTIF(D21:X21,10)</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated games from 10/11/17
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -118,14 +118,20 @@
   <si>
     <t>Best Game</t>
   </si>
+  <si>
+    <t>STDEV</t>
+  </si>
+  <si>
+    <t>Average #10</t>
+  </si>
+  <si>
+    <t>Average #20</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -158,7 +164,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -168,7 +174,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -287,10 +293,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:f>Sheet1!$A$2:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -350,16 +356,25 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Z$2:$Z$21</c:f>
+              <c:f>Sheet1!$Z$2:$Z$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>200</c:v>
                 </c:pt>
@@ -419,6 +434,15 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>146.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>146.52380952380952</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>144.45454545454547</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>145.2608695652174</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -758,16 +782,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2</c:v>
@@ -2075,15 +2099,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2111,15 +2135,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2148,8 +2172,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AA21" totalsRowShown="0">
-  <autoFilter ref="A1:AA21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AA24" totalsRowShown="0">
+  <autoFilter ref="A1:AA24"/>
   <tableColumns count="27">
     <tableColumn id="1" name="Game #">
       <calculatedColumnFormula>A1+1</calculatedColumnFormula>
@@ -2486,7 +2510,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR21"/>
+  <dimension ref="A1:AR24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2722,11 +2746,11 @@
       </c>
       <c r="AC2">
         <f>SUM(Table1[Strikes])</f>
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="AF2">
         <f>COUNTIF(Table1[Strikes],AF1)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AG2">
         <f>COUNTIF(Table1[Strikes],AG1)</f>
@@ -2734,11 +2758,11 @@
       </c>
       <c r="AH2">
         <f>COUNTIF(Table1[Strikes],AH1)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AI2">
         <f>COUNTIF(Table1[Strikes],AI1)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AJ2">
         <f>COUNTIF(Table1[Strikes],AJ1)</f>
@@ -2933,7 +2957,7 @@
       </c>
       <c r="AC4">
         <f>AVERAGE(Table1[Strikes])</f>
-        <v>2.85</v>
+        <v>2.6956521739130435</v>
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
@@ -3018,6 +3042,13 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
+      <c r="AB5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC5">
+        <f>_xlfn.STDEV.P(Table1[Strikes])</f>
+        <v>1.9656790531230113</v>
+      </c>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -3083,6 +3114,13 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="AB6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC6">
+        <f ca="1">AVERAGE(OFFSET(Z2,COUNT(Table1[[#All],[Average]]),0,-10))</f>
+        <v>145.77698852379945</v>
+      </c>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -3163,6 +3201,13 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="AB7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC7">
+        <f ca="1">AVERAGE(OFFSET(Z2,COUNT(Table1[[#All],[Average]]),0,-20))</f>
+        <v>153.58279633523313</v>
+      </c>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -3240,6 +3285,13 @@
         <f t="shared" ref="AA8:AA10" si="3">COUNTIF(D8:X8,10)</f>
         <v>5</v>
       </c>
+      <c r="AB8" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC8">
+        <f>AVERAGE(Table1[Average])</f>
+        <v>157.9198462479462</v>
+      </c>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -3409,7 +3461,7 @@
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" ref="A11:A19" si="4">A10+1</f>
+        <f t="shared" ref="A11:A18" si="4">A10+1</f>
         <v>10</v>
       </c>
       <c r="B11" s="1">
@@ -4260,6 +4312,249 @@
       </c>
       <c r="AA21">
         <f>COUNTIF(D21:X21,10)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f>A21+1</f>
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>42988</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>7</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22">
+        <v>8</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>9</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>10</v>
+      </c>
+      <c r="N22">
+        <v>9</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>7</v>
+      </c>
+      <c r="Q22">
+        <v>3</v>
+      </c>
+      <c r="R22">
+        <v>6</v>
+      </c>
+      <c r="S22">
+        <v>4</v>
+      </c>
+      <c r="T22">
+        <v>9</v>
+      </c>
+      <c r="U22">
+        <v>1</v>
+      </c>
+      <c r="V22">
+        <v>10</v>
+      </c>
+      <c r="W22">
+        <v>6</v>
+      </c>
+      <c r="X22">
+        <v>4</v>
+      </c>
+      <c r="Y22">
+        <v>139</v>
+      </c>
+      <c r="Z22">
+        <f>AVERAGE($Y$2:Y22)</f>
+        <v>146.52380952380952</v>
+      </c>
+      <c r="AA22">
+        <f>COUNTIF(D22:X22,10)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f>A22+1</f>
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>42988</v>
+      </c>
+      <c r="C23">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>6</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>7</v>
+      </c>
+      <c r="J23">
+        <v>9</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>7</v>
+      </c>
+      <c r="M23">
+        <v>2</v>
+      </c>
+      <c r="N23">
+        <v>3</v>
+      </c>
+      <c r="O23">
+        <v>2</v>
+      </c>
+      <c r="P23">
+        <v>6</v>
+      </c>
+      <c r="Q23">
+        <v>3</v>
+      </c>
+      <c r="R23">
+        <v>8</v>
+      </c>
+      <c r="S23">
+        <v>2</v>
+      </c>
+      <c r="T23">
+        <v>6</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>6</v>
+      </c>
+      <c r="W23">
+        <v>2</v>
+      </c>
+      <c r="Y23">
+        <v>101</v>
+      </c>
+      <c r="Z23">
+        <f>AVERAGE($Y$2:Y23)</f>
+        <v>144.45454545454547</v>
+      </c>
+      <c r="AA23">
+        <f>COUNTIF(D23:X23,10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f>A23+1</f>
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>42988</v>
+      </c>
+      <c r="C24">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <v>10</v>
+      </c>
+      <c r="F24">
+        <v>9</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>9</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>8</v>
+      </c>
+      <c r="K24">
+        <v>2</v>
+      </c>
+      <c r="L24">
+        <v>7</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>10</v>
+      </c>
+      <c r="P24">
+        <v>10</v>
+      </c>
+      <c r="R24">
+        <v>9</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>5</v>
+      </c>
+      <c r="U24">
+        <v>1</v>
+      </c>
+      <c r="V24">
+        <v>9</v>
+      </c>
+      <c r="W24">
+        <v>1</v>
+      </c>
+      <c r="X24">
+        <v>9</v>
+      </c>
+      <c r="Y24">
+        <v>163</v>
+      </c>
+      <c r="Z24">
+        <f>AVERAGE($Y$2:Y24)</f>
+        <v>145.2608695652174</v>
+      </c>
+      <c r="AA24">
+        <f>COUNTIF(D24:X24,10)</f>
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added all games up to the 17/9/17
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -119,13 +119,34 @@
     <t>Best Game</t>
   </si>
   <si>
-    <t>STDEV</t>
-  </si>
-  <si>
     <t>Average #10</t>
   </si>
   <si>
     <t>Average #20</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>STDEV strikes</t>
+  </si>
+  <si>
+    <t>Spares</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>Total Spares</t>
+  </si>
+  <si>
+    <t>10th Turkery</t>
+  </si>
+  <si>
+    <t>10th Turkery%</t>
+  </si>
+  <si>
+    <t>Average Spares</t>
   </si>
 </sst>
 </file>
@@ -161,17 +182,91 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="25">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -293,10 +388,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$24</c:f>
+              <c:f>Sheet1!$A$2:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -365,16 +460,37 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Z$2:$Z$24</c:f>
+              <c:f>Sheet1!$Z$2:$Z$31</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>200</c:v>
                 </c:pt>
@@ -443,6 +559,27 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>145.2608695652174</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>145.875</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>145.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>145.61538461538461</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>146.22222222222223</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>147.17857142857142</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>146.44827586206895</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>146.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -549,7 +686,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -729,7 +866,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$AF$1:$AR$1</c:f>
+              <c:f>Sheet1!$AG$1:$AS$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -777,7 +914,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AF$2:$AR$2</c:f>
+              <c:f>Sheet1!$AG$2:$AS$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -785,19 +922,19 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -826,6 +963,84 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-271F-4F91-9627-7EAE15EBB630}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AF$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Spares</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AG$5:$AS$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AFE1-4A66-8DFC-A9F1D1C69735}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -958,6 +1173,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2098,16 +2344,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2134,16 +2380,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2172,41 +2418,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AA24" totalsRowShown="0">
-  <autoFilter ref="A1:AA24"/>
-  <tableColumns count="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AB31" totalsRowShown="0">
+  <autoFilter ref="A1:AB31"/>
+  <tableColumns count="28">
     <tableColumn id="1" name="Game #">
       <calculatedColumnFormula>A1+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Date" dataDxfId="1"/>
+    <tableColumn id="2" name="Date" dataDxfId="24"/>
     <tableColumn id="3" name="Lane"/>
-    <tableColumn id="4" name="1.1"/>
-    <tableColumn id="5" name="1.2"/>
-    <tableColumn id="6" name="2.1"/>
-    <tableColumn id="7" name="2.2"/>
-    <tableColumn id="8" name="3.1"/>
-    <tableColumn id="9" name="3.2"/>
-    <tableColumn id="10" name="4.1"/>
-    <tableColumn id="11" name="4.2"/>
-    <tableColumn id="12" name="5.1"/>
-    <tableColumn id="13" name="5.2"/>
-    <tableColumn id="14" name="6.1"/>
-    <tableColumn id="15" name="6.2"/>
-    <tableColumn id="16" name="7.1"/>
-    <tableColumn id="17" name="7.2"/>
-    <tableColumn id="18" name="8.1"/>
-    <tableColumn id="19" name="8.2"/>
-    <tableColumn id="20" name="9.1"/>
-    <tableColumn id="21" name="9.2"/>
-    <tableColumn id="22" name="10.1"/>
-    <tableColumn id="23" name="10.2"/>
-    <tableColumn id="24" name="10.3"/>
-    <tableColumn id="25" name="Total"/>
-    <tableColumn id="26" name="Average" dataDxfId="0">
+    <tableColumn id="4" name="1.1" dataDxfId="23"/>
+    <tableColumn id="5" name="1.2" dataDxfId="22"/>
+    <tableColumn id="6" name="2.1" dataDxfId="21"/>
+    <tableColumn id="7" name="2.2" dataDxfId="20"/>
+    <tableColumn id="8" name="3.1" dataDxfId="19"/>
+    <tableColumn id="9" name="3.2" dataDxfId="18"/>
+    <tableColumn id="10" name="4.1" dataDxfId="17"/>
+    <tableColumn id="11" name="4.2" dataDxfId="16"/>
+    <tableColumn id="12" name="5.1" dataDxfId="15"/>
+    <tableColumn id="13" name="5.2" dataDxfId="14"/>
+    <tableColumn id="14" name="6.1" dataDxfId="13"/>
+    <tableColumn id="15" name="6.2" dataDxfId="12"/>
+    <tableColumn id="16" name="7.1" dataDxfId="11"/>
+    <tableColumn id="17" name="7.2" dataDxfId="10"/>
+    <tableColumn id="18" name="8.1" dataDxfId="9"/>
+    <tableColumn id="19" name="8.2" dataDxfId="8"/>
+    <tableColumn id="20" name="9.1" dataDxfId="7"/>
+    <tableColumn id="21" name="9.2" dataDxfId="6"/>
+    <tableColumn id="22" name="10.1" dataDxfId="5"/>
+    <tableColumn id="23" name="10.2" dataDxfId="4"/>
+    <tableColumn id="24" name="10.3" dataDxfId="3"/>
+    <tableColumn id="25" name="Total" dataDxfId="2"/>
+    <tableColumn id="26" name="Average" dataDxfId="1">
       <calculatedColumnFormula>AVERAGE($Y$2:Y2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="30" name="Strikes">
-      <calculatedColumnFormula>COUNTIF(D2:X2,10)</calculatedColumnFormula>
+      <calculatedColumnFormula>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="27" name="Spares" dataDxfId="0">
+      <calculatedColumnFormula>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2510,22 +2759,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR24"/>
+  <dimension ref="A1:AS31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="21" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="22" max="24" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -2608,68 +2859,71 @@
         <v>4</v>
       </c>
       <c r="AB1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC1" t="s">
         <v>30</v>
       </c>
-      <c r="AC1">
+      <c r="AD1">
         <f>MAX(Table1[Total])</f>
         <v>259</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>4</v>
       </c>
-      <c r="AF1">
-        <v>0</v>
-      </c>
       <c r="AG1">
-        <f t="shared" ref="AG1:AR1" si="0">AF1+1</f>
+        <v>0</v>
+      </c>
+      <c r="AH1">
+        <f t="shared" ref="AH1:AS1" si="0">AG1+1</f>
         <v>1</v>
       </c>
-      <c r="AH1">
+      <c r="AI1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="AI1">
+      <c r="AJ1">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="AJ1">
+      <c r="AK1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="AK1">
+      <c r="AL1">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="AL1">
+      <c r="AM1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="AM1">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
       <c r="AN1">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AO1">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AP1">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AQ1">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AR1">
         <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AS1">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2679,114 +2933,118 @@
       <c r="C2">
         <v>3</v>
       </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>10</v>
-      </c>
-      <c r="H2">
-        <v>9</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>9</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>8</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>10</v>
-      </c>
-      <c r="P2">
-        <v>7</v>
-      </c>
-      <c r="Q2">
-        <v>3</v>
-      </c>
-      <c r="R2">
-        <v>9</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <v>10</v>
-      </c>
-      <c r="V2">
-        <v>10</v>
-      </c>
-      <c r="W2">
-        <v>10</v>
-      </c>
-      <c r="X2">
-        <v>8</v>
-      </c>
-      <c r="Y2">
+      <c r="D2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3">
+        <v>9</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
+        <v>9</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="3">
+        <v>8</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="3">
+        <v>9</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="X2" s="3">
+        <v>8</v>
+      </c>
+      <c r="Y2" s="3">
         <v>200</v>
       </c>
-      <c r="Z2">
+      <c r="Z2" s="4">
         <f>AVERAGE($Y$2:Y2)</f>
         <v>200</v>
       </c>
       <c r="AA2">
-        <f t="shared" ref="AA2:AA7" si="1">COUNTIF(D2:X2,10)</f>
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
         <v>6</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AB2">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>3</v>
+      </c>
+      <c r="AC2" t="s">
         <v>5</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <f>SUM(Table1[Strikes])</f>
-        <v>62</v>
-      </c>
-      <c r="AF2">
-        <f>COUNTIF(Table1[Strikes],AF1)</f>
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="AG2">
         <f>COUNTIF(Table1[Strikes],AG1)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH2">
         <f>COUNTIF(Table1[Strikes],AH1)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AI2">
         <f>COUNTIF(Table1[Strikes],AI1)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AJ2">
         <f>COUNTIF(Table1[Strikes],AJ1)</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="AK2">
         <f>COUNTIF(Table1[Strikes],AK1)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL2">
         <f>COUNTIF(Table1[Strikes],AL1)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AM2">
         <f>COUNTIF(Table1[Strikes],AM1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN2">
         <f>COUNTIF(Table1[Strikes],AN1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO2">
         <f>COUNTIF(Table1[Strikes],AO1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP2">
         <f>COUNTIF(Table1[Strikes],AP1)</f>
@@ -2800,8 +3058,12 @@
         <f>COUNTIF(Table1[Strikes],AR1)</f>
         <v>0</v>
       </c>
+      <c r="AS2">
+        <f>COUNTIF(Table1[Strikes],AS1)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -2812,79 +3074,87 @@
       <c r="C3">
         <v>3</v>
       </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>7</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3">
-        <v>10</v>
-      </c>
-      <c r="J3">
-        <v>10</v>
-      </c>
-      <c r="L3">
-        <v>8</v>
-      </c>
-      <c r="M3">
+      <c r="D3" s="3">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="3">
+        <v>7</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <v>8</v>
+      </c>
+      <c r="M3" s="3">
         <v>1</v>
       </c>
-      <c r="N3">
-        <v>7</v>
-      </c>
-      <c r="O3">
-        <v>3</v>
-      </c>
-      <c r="P3">
-        <v>7</v>
-      </c>
-      <c r="Q3">
-        <v>3</v>
-      </c>
-      <c r="R3">
-        <v>9</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>10</v>
-      </c>
-      <c r="V3">
-        <v>7</v>
-      </c>
-      <c r="W3">
+      <c r="N3" s="3">
+        <v>7</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="3">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="3">
+        <v>9</v>
+      </c>
+      <c r="S3" s="3">
+        <v>0</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3">
+        <v>7</v>
+      </c>
+      <c r="W3" s="3">
         <v>2</v>
       </c>
-      <c r="Y3">
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3">
         <v>166</v>
       </c>
-      <c r="Z3">
+      <c r="Z3" s="4">
         <f>AVERAGE($Y$2:Y3)</f>
         <v>183</v>
       </c>
       <c r="AA3">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
         <v>3</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AB3">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>4</v>
+      </c>
+      <c r="AC3" t="s">
         <v>6</v>
       </c>
-      <c r="AC3">
+      <c r="AD3">
         <f>MAX(Table1[Strikes])</f>
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A10" si="2">A3+1</f>
+        <f t="shared" ref="A4:A10" si="1">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1">
@@ -2893,166 +3163,286 @@
       <c r="C4">
         <v>15</v>
       </c>
-      <c r="D4">
-        <v>7</v>
-      </c>
-      <c r="E4">
+      <c r="D4" s="3">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3">
+        <v>4</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0</v>
+      </c>
+      <c r="K4" s="3">
         <v>3</v>
       </c>
-      <c r="F4">
-        <v>10</v>
-      </c>
-      <c r="H4">
+      <c r="L4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3">
+        <v>8</v>
+      </c>
+      <c r="O4" s="3">
+        <v>1</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3">
+        <v>7</v>
+      </c>
+      <c r="U4" s="3">
+        <v>2</v>
+      </c>
+      <c r="V4" s="3">
+        <v>5</v>
+      </c>
+      <c r="W4" s="3">
         <v>4</v>
       </c>
-      <c r="I4">
-        <v>6</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>3</v>
-      </c>
-      <c r="L4">
-        <v>10</v>
-      </c>
-      <c r="N4">
-        <v>8</v>
-      </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>10</v>
-      </c>
-      <c r="R4">
-        <v>10</v>
-      </c>
-      <c r="T4">
-        <v>7</v>
-      </c>
-      <c r="U4">
-        <v>2</v>
-      </c>
-      <c r="V4">
-        <v>5</v>
-      </c>
-      <c r="W4">
-        <v>4</v>
-      </c>
-      <c r="Y4">
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3">
         <v>145</v>
       </c>
-      <c r="Z4">
+      <c r="Z4" s="4">
         <f>AVERAGE($Y$2:Y4)</f>
         <v>170.33333333333334</v>
       </c>
       <c r="AA4">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
+        <v>4</v>
+      </c>
+      <c r="AB4">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>2</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD4">
+        <f>AVERAGE(Table1[Strikes])</f>
+        <v>2.8</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <f t="shared" ref="AH4" si="2">AG4+1</f>
+        <v>1</v>
+      </c>
+      <c r="AI4">
+        <f t="shared" ref="AI4" si="3">AH4+1</f>
+        <v>2</v>
+      </c>
+      <c r="AJ4">
+        <f t="shared" ref="AJ4" si="4">AI4+1</f>
+        <v>3</v>
+      </c>
+      <c r="AK4">
+        <f t="shared" ref="AK4" si="5">AJ4+1</f>
+        <v>4</v>
+      </c>
+      <c r="AL4">
+        <f t="shared" ref="AL4" si="6">AK4+1</f>
+        <v>5</v>
+      </c>
+      <c r="AM4">
+        <f t="shared" ref="AM4" si="7">AL4+1</f>
+        <v>6</v>
+      </c>
+      <c r="AN4">
+        <f t="shared" ref="AN4" si="8">AM4+1</f>
+        <v>7</v>
+      </c>
+      <c r="AO4">
+        <f t="shared" ref="AO4" si="9">AN4+1</f>
+        <v>8</v>
+      </c>
+      <c r="AP4">
+        <f t="shared" ref="AP4" si="10">AO4+1</f>
+        <v>9</v>
+      </c>
+      <c r="AQ4">
+        <f t="shared" ref="AQ4" si="11">AP4+1</f>
+        <v>10</v>
+      </c>
+      <c r="AR4">
+        <f t="shared" ref="AR4" si="12">AQ4+1</f>
+        <v>11</v>
+      </c>
+      <c r="AS4">
+        <f t="shared" ref="AS4" si="13">AR4+1</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A5">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AB4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC4">
-        <f>AVERAGE(Table1[Strikes])</f>
-        <v>2.6956521739130435</v>
-      </c>
-    </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
       <c r="B5" s="1">
         <v>42974</v>
       </c>
       <c r="C5">
         <v>15</v>
       </c>
-      <c r="D5">
-        <v>8</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>9</v>
-      </c>
-      <c r="G5">
+      <c r="D5" s="3">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>9</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="3">
+        <v>8</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="3">
+        <v>9</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3">
+        <v>8</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3">
+        <v>6</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5" s="3">
+        <v>9</v>
+      </c>
+      <c r="S5" s="3">
+        <v>0</v>
+      </c>
+      <c r="T5" s="3">
+        <v>3</v>
+      </c>
+      <c r="U5" s="3">
+        <v>5</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="W5" s="3">
+        <v>5</v>
+      </c>
+      <c r="X5" s="3">
         <v>1</v>
       </c>
-      <c r="H5">
-        <v>8</v>
-      </c>
-      <c r="I5">
-        <v>2</v>
-      </c>
-      <c r="J5">
-        <v>9</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>10</v>
-      </c>
-      <c r="N5">
-        <v>8</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>6</v>
-      </c>
-      <c r="Q5">
-        <v>4</v>
-      </c>
-      <c r="R5">
-        <v>9</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>3</v>
-      </c>
-      <c r="U5">
-        <v>5</v>
-      </c>
-      <c r="V5">
-        <v>10</v>
-      </c>
-      <c r="W5">
-        <v>5</v>
-      </c>
-      <c r="X5">
-        <v>1</v>
-      </c>
-      <c r="Y5">
+      <c r="Y5" s="3">
         <v>132</v>
       </c>
-      <c r="Z5">
+      <c r="Z5" s="4">
         <f>AVERAGE($Y$2:Y5)</f>
         <v>160.75</v>
       </c>
       <c r="AA5">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
+        <v>2</v>
+      </c>
+      <c r="AB5">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>3</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD5">
+        <f>_xlfn.STDEV.P(Table1[Strikes])</f>
+        <v>1.8147543451754933</v>
+      </c>
+      <c r="AG5">
+        <f>COUNTIF(Table1[Spares],AG4)</f>
+        <v>1</v>
+      </c>
+      <c r="AH5">
+        <f>COUNTIF(Table1[Spares],AH4)</f>
+        <v>1</v>
+      </c>
+      <c r="AI5">
+        <f>COUNTIF(Table1[Spares],AI4)</f>
+        <v>13</v>
+      </c>
+      <c r="AJ5">
+        <f>COUNTIF(Table1[Spares],AJ4)</f>
+        <v>7</v>
+      </c>
+      <c r="AK5">
+        <f>COUNTIF(Table1[Spares],AK4)</f>
+        <v>6</v>
+      </c>
+      <c r="AL5">
+        <f>COUNTIF(Table1[Spares],AL4)</f>
+        <v>2</v>
+      </c>
+      <c r="AM5">
+        <f>COUNTIF(Table1[Spares],AM4)</f>
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <f>COUNTIF(Table1[Spares],AN4)</f>
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <f>COUNTIF(Table1[Spares],AO4)</f>
+        <v>0</v>
+      </c>
+      <c r="AP5">
+        <f>COUNTIF(Table1[Spares],AP4)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <f>COUNTIF(Table1[Spares],AQ4)</f>
+        <v>0</v>
+      </c>
+      <c r="AR5">
+        <f>COUNTIF(Table1[Spares],AR4)</f>
+        <v>0</v>
+      </c>
+      <c r="AS5">
+        <f>COUNTIF(Table1[Spares],AS4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A6">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC5">
-        <f>_xlfn.STDEV.P(Table1[Strikes])</f>
-        <v>1.9656790531230113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="B6" s="1">
@@ -3061,70 +3451,81 @@
       <c r="C6">
         <v>15</v>
       </c>
-      <c r="D6">
-        <v>9</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>9</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>10</v>
-      </c>
-      <c r="J6">
-        <v>10</v>
-      </c>
-      <c r="L6">
-        <v>10</v>
-      </c>
-      <c r="N6">
-        <v>10</v>
-      </c>
-      <c r="P6">
-        <v>10</v>
-      </c>
-      <c r="R6">
-        <v>10</v>
-      </c>
-      <c r="T6">
-        <v>10</v>
-      </c>
-      <c r="V6">
-        <v>10</v>
-      </c>
-      <c r="W6">
+      <c r="D6" s="3">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="3">
+        <v>9</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="W6" s="3">
         <v>2</v>
       </c>
-      <c r="X6">
+      <c r="X6" s="3">
         <v>6</v>
       </c>
-      <c r="Y6">
+      <c r="Y6" s="3">
         <v>259</v>
       </c>
-      <c r="Z6">
+      <c r="Z6" s="4">
         <f>AVERAGE($Y$2:Y6)</f>
         <v>180.4</v>
       </c>
       <c r="AA6">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
+        <v>8</v>
+      </c>
+      <c r="AB6">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>2</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD6">
+        <f>SUM(Table1[Spares])</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A7">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC6">
-        <f ca="1">AVERAGE(OFFSET(Z2,COUNT(Table1[[#All],[Average]]),0,-10))</f>
-        <v>145.77698852379945</v>
-      </c>
-    </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="B7" s="1">
@@ -3133,85 +3534,91 @@
       <c r="C7">
         <v>5</v>
       </c>
-      <c r="D7">
-        <v>7</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>8</v>
-      </c>
-      <c r="G7">
-        <v>2</v>
-      </c>
-      <c r="H7">
-        <v>8</v>
-      </c>
-      <c r="I7">
+      <c r="D7" s="3">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>8</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="3">
+        <v>8</v>
+      </c>
+      <c r="I7" s="3">
         <v>1</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="3">
         <v>4</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="3">
         <v>3</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="3">
         <v>1</v>
       </c>
-      <c r="M7">
-        <v>9</v>
-      </c>
-      <c r="N7">
+      <c r="M7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N7" s="3">
         <v>6</v>
       </c>
-      <c r="O7">
-        <v>4</v>
-      </c>
-      <c r="P7">
-        <v>10</v>
-      </c>
-      <c r="R7">
+      <c r="O7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3">
         <v>6</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="3">
         <v>3</v>
       </c>
-      <c r="T7">
-        <v>8</v>
-      </c>
-      <c r="U7">
-        <v>2</v>
-      </c>
-      <c r="V7">
-        <v>9</v>
-      </c>
-      <c r="W7">
-        <v>0</v>
-      </c>
-      <c r="Y7">
+      <c r="T7" s="3">
+        <v>8</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V7" s="3">
+        <v>9</v>
+      </c>
+      <c r="W7" s="3">
+        <v>0</v>
+      </c>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3">
         <v>133</v>
       </c>
-      <c r="Z7">
+      <c r="Z7" s="4">
         <f>AVERAGE($Y$2:Y7)</f>
         <v>172.5</v>
       </c>
       <c r="AA7">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
+        <v>1</v>
+      </c>
+      <c r="AB7">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>4</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD7">
+        <f>AVERAGE(Table1[Spares])</f>
+        <v>2.7333333333333334</v>
+      </c>
+    </row>
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A8">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC7">
-        <f ca="1">AVERAGE(OFFSET(Z2,COUNT(Table1[[#All],[Average]]),0,-20))</f>
-        <v>153.58279633523313</v>
-      </c>
-    </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="B8" s="1">
@@ -3220,82 +3627,89 @@
       <c r="C8">
         <v>5</v>
       </c>
-      <c r="D8">
-        <v>7</v>
-      </c>
-      <c r="E8">
+      <c r="D8" s="3">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="3">
+        <v>9</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="3">
+        <v>8</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3">
+        <v>5</v>
+      </c>
+      <c r="K8" s="3">
         <v>3</v>
       </c>
-      <c r="F8">
-        <v>9</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>8</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>5</v>
-      </c>
-      <c r="K8">
+      <c r="L8" s="3">
+        <v>6</v>
+      </c>
+      <c r="M8" s="3">
         <v>3</v>
       </c>
-      <c r="L8">
-        <v>6</v>
-      </c>
-      <c r="M8">
-        <v>3</v>
-      </c>
-      <c r="N8">
-        <v>10</v>
-      </c>
-      <c r="P8">
-        <v>10</v>
-      </c>
-      <c r="R8">
-        <v>7</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>10</v>
-      </c>
-      <c r="V8">
-        <v>10</v>
-      </c>
-      <c r="W8">
-        <v>10</v>
-      </c>
-      <c r="X8">
-        <v>7</v>
-      </c>
-      <c r="Y8">
+      <c r="N8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3">
+        <v>7</v>
+      </c>
+      <c r="S8" s="3">
+        <v>0</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="X8" s="3">
+        <v>7</v>
+      </c>
+      <c r="Y8" s="3">
         <v>171</v>
       </c>
-      <c r="Z8">
+      <c r="Z8" s="4">
         <f>AVERAGE($Y$2:Y8)</f>
         <v>172.28571428571428</v>
       </c>
       <c r="AA8">
-        <f t="shared" ref="AA8:AA10" si="3">COUNTIF(D8:X8,10)</f>
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
         <v>5</v>
       </c>
-      <c r="AB8" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC8">
-        <f>AVERAGE(Table1[Average])</f>
-        <v>157.9198462479462</v>
+      <c r="AB8">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>2</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD8">
+        <f ca="1">AVERAGE(OFFSET(Z2,COUNT(Table1[[#All],[Average]]),0,-10))</f>
+        <v>145.83942990533444</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B9" s="1">
@@ -3304,81 +3718,93 @@
       <c r="C9">
         <v>5</v>
       </c>
-      <c r="D9">
-        <v>9</v>
-      </c>
-      <c r="E9">
+      <c r="D9" s="3">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="3">
+        <v>8</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="3">
+        <v>6</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
+        <v>9</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
+        <v>7</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3">
+        <v>8</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>0</v>
+      </c>
+      <c r="R9" s="3">
+        <v>0</v>
+      </c>
+      <c r="S9" s="3">
+        <v>9</v>
+      </c>
+      <c r="T9" s="3">
+        <v>6</v>
+      </c>
+      <c r="U9" s="3">
         <v>1</v>
       </c>
-      <c r="F9">
-        <v>8</v>
-      </c>
-      <c r="G9">
-        <v>2</v>
-      </c>
-      <c r="H9">
-        <v>6</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>9</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>7</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>10</v>
-      </c>
-      <c r="P9">
-        <v>8</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>9</v>
-      </c>
-      <c r="T9">
-        <v>6</v>
-      </c>
-      <c r="U9">
-        <v>1</v>
-      </c>
-      <c r="V9">
-        <v>10</v>
-      </c>
-      <c r="W9">
-        <v>10</v>
-      </c>
-      <c r="X9">
-        <v>7</v>
-      </c>
-      <c r="Y9">
+      <c r="V9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="X9" s="3">
+        <v>7</v>
+      </c>
+      <c r="Y9" s="3">
         <v>125</v>
       </c>
-      <c r="Z9">
+      <c r="Z9" s="4">
         <f>AVERAGE($Y$2:Y9)</f>
         <v>166.375</v>
       </c>
       <c r="AA9">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
         <v>3</v>
       </c>
+      <c r="AB9">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>2</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD9">
+        <f ca="1">AVERAGE(OFFSET(Z2,COUNT(Table1[[#All],[Average]]),0,-20))</f>
+        <v>146.59369226527605</v>
+      </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B10" s="1">
@@ -3387,81 +3813,93 @@
       <c r="C10">
         <v>5</v>
       </c>
-      <c r="D10">
-        <v>9</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>7</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
+      <c r="D10" s="3">
+        <v>9</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>7</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3">
         <v>6</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="3">
         <v>3</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="3">
         <v>5</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="3">
         <v>3</v>
       </c>
-      <c r="L10">
-        <v>7</v>
-      </c>
-      <c r="M10">
+      <c r="L10" s="3">
+        <v>7</v>
+      </c>
+      <c r="M10" s="3">
         <v>2</v>
       </c>
-      <c r="N10">
-        <v>8</v>
-      </c>
-      <c r="O10">
+      <c r="N10" s="3">
+        <v>8</v>
+      </c>
+      <c r="O10" s="3">
         <v>1</v>
       </c>
-      <c r="P10">
-        <v>9</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>8</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <v>8</v>
-      </c>
-      <c r="U10">
+      <c r="P10" s="3">
+        <v>9</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>0</v>
+      </c>
+      <c r="R10" s="3">
+        <v>8</v>
+      </c>
+      <c r="S10" s="3">
+        <v>0</v>
+      </c>
+      <c r="T10" s="3">
+        <v>8</v>
+      </c>
+      <c r="U10" s="3">
         <v>1</v>
       </c>
-      <c r="V10">
+      <c r="V10" s="3">
         <v>6</v>
       </c>
-      <c r="W10">
+      <c r="W10" s="3">
         <v>3</v>
       </c>
-      <c r="Y10">
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3">
         <v>86</v>
       </c>
-      <c r="Z10">
+      <c r="Z10" s="4">
         <f>AVERAGE($Y$2:Y10)</f>
         <v>157.44444444444446</v>
       </c>
       <c r="AA10">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>0</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD10">
+        <f>AVERAGE(Table1[Average])</f>
+        <v>155.16653059436703</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" ref="A11:A18" si="4">A10+1</f>
+        <f t="shared" ref="A11:A18" si="14">A10+1</f>
         <v>10</v>
       </c>
       <c r="B11" s="1">
@@ -3470,78 +3908,91 @@
       <c r="C11">
         <v>8</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>2</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>6</v>
       </c>
-      <c r="F11">
-        <v>8</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>7</v>
-      </c>
-      <c r="I11">
+      <c r="F11" s="3">
+        <v>8</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3">
+        <v>7</v>
+      </c>
+      <c r="I11" s="3">
         <v>1</v>
       </c>
-      <c r="J11">
-        <v>9</v>
-      </c>
-      <c r="K11">
+      <c r="J11" s="3">
+        <v>9</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L11" s="3">
+        <v>8</v>
+      </c>
+      <c r="M11" s="3">
         <v>1</v>
       </c>
-      <c r="L11">
-        <v>8</v>
-      </c>
-      <c r="M11">
+      <c r="N11" s="3">
+        <v>8</v>
+      </c>
+      <c r="O11" s="3">
         <v>1</v>
       </c>
-      <c r="N11">
-        <v>8</v>
-      </c>
-      <c r="O11">
-        <v>1</v>
-      </c>
-      <c r="P11">
-        <v>7</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
+      <c r="P11" s="3">
+        <v>7</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>0</v>
+      </c>
+      <c r="R11" s="3">
         <v>4</v>
       </c>
-      <c r="S11">
+      <c r="S11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3">
         <v>6</v>
       </c>
-      <c r="T11">
-        <v>10</v>
-      </c>
-      <c r="V11">
-        <v>6</v>
-      </c>
-      <c r="W11">
+      <c r="W11" s="3">
         <v>3</v>
       </c>
-      <c r="Y11">
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3">
         <v>132</v>
       </c>
-      <c r="Z11">
+      <c r="Z11" s="4">
         <f>AVERAGE($Y$2:Y11)</f>
         <v>154.9</v>
       </c>
       <c r="AA11">
-        <f>COUNTIF(D11:X11,10)</f>
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
         <v>1</v>
       </c>
+      <c r="AB11">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>2</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD11">
+        <f>COUNTIFS(Table1[10.1],"=x",Table1[10.2],"=x",Table1[10.3],"=x")</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>11</v>
       </c>
       <c r="B12" s="1">
@@ -3550,78 +4001,91 @@
       <c r="C12">
         <v>8</v>
       </c>
-      <c r="D12">
-        <v>8</v>
-      </c>
-      <c r="E12">
+      <c r="D12" s="3">
+        <v>8</v>
+      </c>
+      <c r="E12" s="3">
         <v>1</v>
       </c>
-      <c r="F12">
-        <v>8</v>
-      </c>
-      <c r="G12">
+      <c r="F12" s="3">
+        <v>8</v>
+      </c>
+      <c r="G12" s="3">
         <v>1</v>
       </c>
-      <c r="H12">
-        <v>7</v>
-      </c>
-      <c r="I12">
+      <c r="H12" s="3">
+        <v>7</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="3">
+        <v>7</v>
+      </c>
+      <c r="K12" s="3">
         <v>3</v>
       </c>
-      <c r="J12">
-        <v>7</v>
-      </c>
-      <c r="K12">
+      <c r="L12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3">
+        <v>8</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P12" s="3">
         <v>3</v>
       </c>
-      <c r="L12">
-        <v>10</v>
-      </c>
-      <c r="N12">
-        <v>8</v>
-      </c>
-      <c r="O12">
-        <v>2</v>
-      </c>
-      <c r="P12">
+      <c r="Q12" s="3">
+        <v>6</v>
+      </c>
+      <c r="R12" s="3">
+        <v>6</v>
+      </c>
+      <c r="S12" s="3">
         <v>3</v>
       </c>
-      <c r="Q12">
-        <v>6</v>
-      </c>
-      <c r="R12">
-        <v>6</v>
-      </c>
-      <c r="S12">
-        <v>3</v>
-      </c>
-      <c r="T12">
-        <v>7</v>
-      </c>
-      <c r="U12">
+      <c r="T12" s="3">
+        <v>7</v>
+      </c>
+      <c r="U12" s="3">
         <v>1</v>
       </c>
-      <c r="V12">
+      <c r="V12" s="3">
         <v>5</v>
       </c>
-      <c r="W12">
+      <c r="W12" s="3">
         <v>1</v>
       </c>
-      <c r="Y12">
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3">
         <v>120</v>
       </c>
-      <c r="Z12">
+      <c r="Z12" s="4">
         <f>AVERAGE($Y$2:Y12)</f>
         <v>151.72727272727272</v>
       </c>
       <c r="AA12">
-        <f>COUNTIF(E12:X12,10)</f>
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
         <v>1</v>
       </c>
+      <c r="AB12">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>2</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD12">
+        <f>100*AD11/MAX(Table1[Game '#])</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>12</v>
       </c>
       <c r="B13" s="1">
@@ -3630,78 +4094,84 @@
       <c r="C13">
         <v>7</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <v>6</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="3">
         <v>3</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="3">
         <v>6</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="3">
         <v>3</v>
       </c>
-      <c r="H13">
-        <v>9</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
-        <v>8</v>
-      </c>
-      <c r="K13">
+      <c r="H13" s="3">
+        <v>9</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" s="3">
+        <v>8</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L13" s="3">
+        <v>6</v>
+      </c>
+      <c r="M13" s="3">
+        <v>3</v>
+      </c>
+      <c r="N13" s="3">
+        <v>7</v>
+      </c>
+      <c r="O13" s="3">
         <v>2</v>
       </c>
-      <c r="L13">
+      <c r="P13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3">
+        <v>9</v>
+      </c>
+      <c r="S13" s="3">
+        <v>0</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3">
+        <v>9</v>
+      </c>
+      <c r="W13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X13" s="3">
         <v>6</v>
       </c>
-      <c r="M13">
-        <v>3</v>
-      </c>
-      <c r="N13">
-        <v>7</v>
-      </c>
-      <c r="O13">
-        <v>2</v>
-      </c>
-      <c r="P13">
-        <v>10</v>
-      </c>
-      <c r="R13">
-        <v>9</v>
-      </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
-      <c r="T13">
-        <v>10</v>
-      </c>
-      <c r="V13">
-        <v>9</v>
-      </c>
-      <c r="W13">
-        <v>1</v>
-      </c>
-      <c r="X13">
-        <v>6</v>
-      </c>
-      <c r="Y13">
+      <c r="Y13" s="3">
         <v>134</v>
       </c>
-      <c r="Z13">
+      <c r="Z13" s="4">
         <f>AVERAGE($Y$2:Y13)</f>
         <v>150.25</v>
       </c>
       <c r="AA13">
-        <f t="shared" ref="AA13:AA18" si="5">COUNTIF(D13:X13,10)</f>
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
         <v>2</v>
       </c>
+      <c r="AB13">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>3</v>
+      </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>13</v>
       </c>
       <c r="B14" s="1">
@@ -3710,69 +4180,78 @@
       <c r="C14">
         <v>7</v>
       </c>
-      <c r="D14">
-        <v>10</v>
-      </c>
-      <c r="F14">
-        <v>7</v>
-      </c>
-      <c r="G14">
+      <c r="D14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3">
+        <v>7</v>
+      </c>
+      <c r="G14" s="3">
         <v>2</v>
       </c>
-      <c r="H14">
-        <v>10</v>
-      </c>
-      <c r="J14">
-        <v>10</v>
-      </c>
-      <c r="L14">
-        <v>9</v>
-      </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
-      <c r="N14">
-        <v>7</v>
-      </c>
-      <c r="O14">
+      <c r="H14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3">
+        <v>9</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N14" s="3">
+        <v>7</v>
+      </c>
+      <c r="O14" s="3">
         <v>2</v>
       </c>
-      <c r="P14">
-        <v>8</v>
-      </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-      <c r="R14">
-        <v>9</v>
-      </c>
-      <c r="S14">
-        <v>1</v>
-      </c>
-      <c r="T14">
-        <v>10</v>
-      </c>
-      <c r="V14">
+      <c r="P14" s="3">
+        <v>8</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>0</v>
+      </c>
+      <c r="R14" s="3">
+        <v>9</v>
+      </c>
+      <c r="S14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3">
         <v>6</v>
       </c>
-      <c r="W14">
+      <c r="W14" s="3">
         <v>2</v>
       </c>
-      <c r="Y14">
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3">
         <v>157</v>
       </c>
-      <c r="Z14">
+      <c r="Z14" s="4">
         <f>AVERAGE($Y$2:Y14)</f>
         <v>150.76923076923077</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="5"/>
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
         <v>4</v>
       </c>
+      <c r="AB14">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>2</v>
+      </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>14</v>
       </c>
       <c r="B15" s="1">
@@ -3781,75 +4260,82 @@
       <c r="C15">
         <v>7</v>
       </c>
-      <c r="D15">
-        <v>9</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>7</v>
-      </c>
-      <c r="G15">
+      <c r="D15" s="3">
+        <v>9</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>7</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="3">
+        <v>8</v>
+      </c>
+      <c r="I15" s="3">
+        <v>1</v>
+      </c>
+      <c r="J15" s="3">
+        <v>7</v>
+      </c>
+      <c r="K15" s="3">
+        <v>1</v>
+      </c>
+      <c r="L15" s="3">
+        <v>5</v>
+      </c>
+      <c r="M15" s="3">
+        <v>4</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3">
+        <v>8</v>
+      </c>
+      <c r="S15" s="3">
+        <v>0</v>
+      </c>
+      <c r="T15" s="3">
+        <v>8</v>
+      </c>
+      <c r="U15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V15" s="3">
+        <v>6</v>
+      </c>
+      <c r="W15" s="3">
         <v>3</v>
       </c>
-      <c r="H15">
-        <v>8</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>7</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <v>5</v>
-      </c>
-      <c r="M15">
-        <v>4</v>
-      </c>
-      <c r="N15">
-        <v>10</v>
-      </c>
-      <c r="P15">
-        <v>10</v>
-      </c>
-      <c r="R15">
-        <v>8</v>
-      </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
-      <c r="T15">
-        <v>8</v>
-      </c>
-      <c r="U15">
-        <v>2</v>
-      </c>
-      <c r="V15">
-        <v>6</v>
-      </c>
-      <c r="W15">
-        <v>3</v>
-      </c>
-      <c r="Y15">
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3">
         <v>132</v>
       </c>
-      <c r="Z15">
+      <c r="Z15" s="4">
         <f>AVERAGE($Y$2:Y15)</f>
         <v>149.42857142857142</v>
       </c>
       <c r="AA15">
-        <f t="shared" si="5"/>
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
         <v>2</v>
       </c>
+      <c r="AB15">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>2</v>
+      </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>15</v>
       </c>
       <c r="B16" s="1">
@@ -3858,75 +4344,82 @@
       <c r="C16">
         <v>11</v>
       </c>
-      <c r="D16">
-        <v>9</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>10</v>
-      </c>
-      <c r="H16">
-        <v>9</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>10</v>
-      </c>
-      <c r="L16">
+      <c r="D16" s="3">
+        <v>9</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3">
+        <v>9</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3">
         <v>6</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="3">
         <v>1</v>
       </c>
-      <c r="N16">
-        <v>7</v>
-      </c>
-      <c r="O16">
+      <c r="N16" s="3">
+        <v>7</v>
+      </c>
+      <c r="O16" s="3">
         <v>1</v>
       </c>
-      <c r="P16">
-        <v>8</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16">
-        <v>9</v>
-      </c>
-      <c r="S16">
-        <v>0</v>
-      </c>
-      <c r="T16">
-        <v>10</v>
-      </c>
-      <c r="V16">
-        <v>8</v>
-      </c>
-      <c r="W16">
-        <v>2</v>
-      </c>
-      <c r="X16">
-        <v>7</v>
-      </c>
-      <c r="Y16">
+      <c r="P16" s="3">
+        <v>8</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>0</v>
+      </c>
+      <c r="R16" s="3">
+        <v>9</v>
+      </c>
+      <c r="S16" s="3">
+        <v>0</v>
+      </c>
+      <c r="T16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3">
+        <v>8</v>
+      </c>
+      <c r="W16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X16" s="3">
+        <v>7</v>
+      </c>
+      <c r="Y16" s="3">
         <v>123</v>
       </c>
-      <c r="Z16">
+      <c r="Z16" s="4">
         <f>AVERAGE($Y$2:Y16)</f>
         <v>147.66666666666666</v>
       </c>
       <c r="AA16">
-        <f t="shared" si="5"/>
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
         <v>3</v>
       </c>
+      <c r="AB16">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>16</v>
       </c>
       <c r="B17" s="1">
@@ -3935,81 +4428,86 @@
       <c r="C17">
         <v>11</v>
       </c>
-      <c r="D17">
-        <v>8</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>8</v>
-      </c>
-      <c r="G17">
+      <c r="D17" s="3">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>8</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="3">
+        <v>6</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0</v>
+      </c>
+      <c r="J17" s="3">
+        <v>7</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0</v>
+      </c>
+      <c r="L17" s="3">
+        <v>8</v>
+      </c>
+      <c r="M17" s="3">
+        <v>0</v>
+      </c>
+      <c r="N17" s="3">
+        <v>3</v>
+      </c>
+      <c r="O17" s="3">
+        <v>6</v>
+      </c>
+      <c r="P17" s="3">
+        <v>8</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>1</v>
+      </c>
+      <c r="R17" s="3">
+        <v>8</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T17" s="3">
+        <v>7</v>
+      </c>
+      <c r="U17" s="3">
         <v>2</v>
       </c>
-      <c r="H17">
+      <c r="V17" s="3">
         <v>6</v>
       </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>7</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>8</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17">
-        <v>3</v>
-      </c>
-      <c r="O17">
-        <v>6</v>
-      </c>
-      <c r="P17">
-        <v>8</v>
-      </c>
-      <c r="Q17">
-        <v>1</v>
-      </c>
-      <c r="R17">
-        <v>8</v>
-      </c>
-      <c r="S17">
-        <v>2</v>
-      </c>
-      <c r="T17">
-        <v>7</v>
-      </c>
-      <c r="U17">
-        <v>2</v>
-      </c>
-      <c r="V17">
-        <v>6</v>
-      </c>
-      <c r="W17">
-        <v>0</v>
-      </c>
-      <c r="Y17">
+      <c r="W17" s="3">
+        <v>0</v>
+      </c>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3">
         <v>95</v>
       </c>
-      <c r="Z17">
+      <c r="Z17" s="4">
         <f>AVERAGE($Y$2:Y17)</f>
         <v>144.375</v>
       </c>
       <c r="AA17">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
+        <v>0</v>
+      </c>
+      <c r="AB17">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>17</v>
       </c>
       <c r="B18" s="1">
@@ -4018,78 +4516,84 @@
       <c r="C18">
         <v>11</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="3">
         <v>5</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="3">
         <v>4</v>
       </c>
-      <c r="F18">
-        <v>8</v>
-      </c>
-      <c r="G18">
-        <v>2</v>
-      </c>
-      <c r="H18">
-        <v>8</v>
-      </c>
-      <c r="I18">
-        <v>2</v>
-      </c>
-      <c r="J18">
-        <v>10</v>
-      </c>
-      <c r="L18">
+      <c r="F18" s="3">
+        <v>8</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H18" s="3">
+        <v>8</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3">
         <v>3</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="3">
         <v>5</v>
       </c>
-      <c r="N18">
-        <v>9</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
-        <v>8</v>
-      </c>
-      <c r="Q18">
+      <c r="N18" s="3">
+        <v>9</v>
+      </c>
+      <c r="O18" s="3">
+        <v>0</v>
+      </c>
+      <c r="P18" s="3">
+        <v>8</v>
+      </c>
+      <c r="Q18" s="3">
         <v>1</v>
       </c>
-      <c r="R18">
-        <v>9</v>
-      </c>
-      <c r="S18">
+      <c r="R18" s="3">
+        <v>9</v>
+      </c>
+      <c r="S18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T18" s="3">
         <v>1</v>
       </c>
-      <c r="T18">
-        <v>1</v>
-      </c>
-      <c r="U18">
-        <v>9</v>
-      </c>
-      <c r="V18">
+      <c r="U18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V18" s="3">
         <v>6</v>
       </c>
-      <c r="W18">
+      <c r="W18" s="3">
         <v>3</v>
       </c>
-      <c r="Y18">
+      <c r="X18" s="3"/>
+      <c r="Y18" s="3">
         <v>127</v>
       </c>
-      <c r="Z18">
+      <c r="Z18" s="4">
         <f>AVERAGE($Y$2:Y18)</f>
         <v>143.35294117647058</v>
       </c>
       <c r="AA18">
-        <f t="shared" si="5"/>
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
         <v>1</v>
       </c>
+      <c r="AB18">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>4</v>
+      </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>A18+1</f>
+        <f t="shared" ref="A19:A24" si="15">A18+1</f>
         <v>18</v>
       </c>
       <c r="B19" s="2">
@@ -4098,69 +4602,78 @@
       <c r="C19">
         <v>11</v>
       </c>
-      <c r="D19">
-        <v>7</v>
-      </c>
-      <c r="E19">
-        <v>3</v>
-      </c>
-      <c r="F19">
-        <v>10</v>
-      </c>
-      <c r="H19">
-        <v>10</v>
-      </c>
-      <c r="J19">
-        <v>10</v>
-      </c>
-      <c r="L19">
-        <v>7</v>
-      </c>
-      <c r="M19">
-        <v>3</v>
-      </c>
-      <c r="N19">
+      <c r="D19" s="3">
+        <v>7</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3">
+        <v>7</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N19" s="3">
         <v>2</v>
       </c>
-      <c r="O19">
-        <v>8</v>
-      </c>
-      <c r="P19">
-        <v>10</v>
-      </c>
-      <c r="R19">
-        <v>7</v>
-      </c>
-      <c r="S19">
-        <v>3</v>
-      </c>
-      <c r="T19">
-        <v>10</v>
-      </c>
-      <c r="V19">
-        <v>9</v>
-      </c>
-      <c r="W19">
-        <v>1</v>
-      </c>
-      <c r="X19">
+      <c r="O19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3">
+        <v>7</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3">
+        <v>9</v>
+      </c>
+      <c r="W19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X19" s="3">
         <v>5</v>
       </c>
-      <c r="Y19">
+      <c r="Y19" s="3">
         <v>204</v>
       </c>
-      <c r="Z19">
+      <c r="Z19" s="4">
         <f>AVERAGE($Y$2:Y19)</f>
         <v>146.72222222222223</v>
       </c>
       <c r="AA19">
-        <f>COUNTIF(D19:X19,10)</f>
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
         <v>5</v>
       </c>
+      <c r="AB19">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>5</v>
+      </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>A19+1</f>
+        <f t="shared" si="15"/>
         <v>19</v>
       </c>
       <c r="B20" s="2">
@@ -4169,75 +4682,82 @@
       <c r="C20">
         <v>11</v>
       </c>
-      <c r="D20">
-        <v>7</v>
-      </c>
-      <c r="E20">
+      <c r="D20" s="3">
+        <v>7</v>
+      </c>
+      <c r="E20" s="3">
         <v>2</v>
       </c>
-      <c r="F20">
-        <v>10</v>
-      </c>
-      <c r="H20">
-        <v>10</v>
-      </c>
-      <c r="J20">
-        <v>9</v>
-      </c>
-      <c r="K20">
+      <c r="F20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3">
+        <v>9</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3">
+        <v>9</v>
+      </c>
+      <c r="O20" s="3">
+        <v>0</v>
+      </c>
+      <c r="P20" s="3">
+        <v>8</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>0</v>
+      </c>
+      <c r="R20" s="3">
+        <v>8</v>
+      </c>
+      <c r="S20" s="3">
         <v>1</v>
       </c>
-      <c r="L20">
-        <v>10</v>
-      </c>
-      <c r="N20">
-        <v>9</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20">
-        <v>8</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20">
-        <v>8</v>
-      </c>
-      <c r="S20">
-        <v>1</v>
-      </c>
-      <c r="T20">
-        <v>9</v>
-      </c>
-      <c r="U20">
-        <v>0</v>
-      </c>
-      <c r="V20">
-        <v>7</v>
-      </c>
-      <c r="W20">
-        <v>3</v>
-      </c>
-      <c r="X20">
+      <c r="T20" s="3">
+        <v>9</v>
+      </c>
+      <c r="U20" s="3">
+        <v>0</v>
+      </c>
+      <c r="V20" s="3">
+        <v>7</v>
+      </c>
+      <c r="W20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X20" s="3">
         <v>5</v>
       </c>
-      <c r="Y20">
+      <c r="Y20" s="3">
         <v>147</v>
       </c>
-      <c r="Z20">
+      <c r="Z20" s="4">
         <f>AVERAGE($Y$2:Y20)</f>
         <v>146.73684210526315</v>
       </c>
       <c r="AA20">
-        <f>COUNTIF(D20:X20,10)</f>
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
         <v>3</v>
       </c>
+      <c r="AB20">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>2</v>
+      </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f>A20+1</f>
+        <f t="shared" si="15"/>
         <v>20</v>
       </c>
       <c r="B21" s="2">
@@ -4246,78 +4766,84 @@
       <c r="C21">
         <v>11</v>
       </c>
-      <c r="D21">
-        <v>8</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
+      <c r="D21" s="3">
+        <v>8</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
         <v>3</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="3">
         <v>6</v>
       </c>
-      <c r="H21">
-        <v>9</v>
-      </c>
-      <c r="I21">
+      <c r="H21" s="3">
+        <v>9</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3">
+        <v>7</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N21" s="3">
+        <v>7</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3">
+        <v>8</v>
+      </c>
+      <c r="S21" s="3">
         <v>1</v>
       </c>
-      <c r="J21">
-        <v>10</v>
-      </c>
-      <c r="L21">
-        <v>7</v>
-      </c>
-      <c r="M21">
+      <c r="T21" s="3">
+        <v>5</v>
+      </c>
+      <c r="U21" s="3">
+        <v>4</v>
+      </c>
+      <c r="V21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="W21" s="3">
+        <v>6</v>
+      </c>
+      <c r="X21" s="3">
         <v>3</v>
       </c>
-      <c r="N21">
-        <v>7</v>
-      </c>
-      <c r="O21">
-        <v>3</v>
-      </c>
-      <c r="P21">
-        <v>10</v>
-      </c>
-      <c r="R21">
-        <v>8</v>
-      </c>
-      <c r="S21">
-        <v>1</v>
-      </c>
-      <c r="T21">
-        <v>5</v>
-      </c>
-      <c r="U21">
-        <v>4</v>
-      </c>
-      <c r="V21">
-        <v>10</v>
-      </c>
-      <c r="W21">
-        <v>6</v>
-      </c>
-      <c r="X21">
-        <v>3</v>
-      </c>
-      <c r="Y21">
+      <c r="Y21" s="3">
         <v>150</v>
       </c>
-      <c r="Z21">
+      <c r="Z21" s="4">
         <f>AVERAGE($Y$2:Y21)</f>
         <v>146.9</v>
       </c>
       <c r="AA21">
-        <f>COUNTIF(D21:X21,10)</f>
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
         <v>3</v>
       </c>
+      <c r="AB21">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>3</v>
+      </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>A21+1</f>
+        <f t="shared" si="15"/>
         <v>21</v>
       </c>
       <c r="B22" s="2">
@@ -4326,81 +4852,86 @@
       <c r="C22">
         <v>7</v>
       </c>
-      <c r="D22">
-        <v>8</v>
-      </c>
-      <c r="E22">
+      <c r="D22" s="3">
+        <v>8</v>
+      </c>
+      <c r="E22" s="3">
         <v>1</v>
       </c>
-      <c r="F22">
-        <v>7</v>
-      </c>
-      <c r="G22">
+      <c r="F22" s="3">
+        <v>7</v>
+      </c>
+      <c r="G22" s="3">
         <v>2</v>
       </c>
-      <c r="H22">
-        <v>8</v>
-      </c>
-      <c r="I22">
+      <c r="H22" s="3">
+        <v>8</v>
+      </c>
+      <c r="I22" s="3">
         <v>1</v>
       </c>
-      <c r="J22">
-        <v>9</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>10</v>
-      </c>
-      <c r="N22">
-        <v>9</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22">
-        <v>7</v>
-      </c>
-      <c r="Q22">
-        <v>3</v>
-      </c>
-      <c r="R22">
+      <c r="J22" s="3">
+        <v>9</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3">
+        <v>9</v>
+      </c>
+      <c r="O22" s="3">
+        <v>0</v>
+      </c>
+      <c r="P22" s="3">
+        <v>7</v>
+      </c>
+      <c r="Q22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R22" s="3">
         <v>6</v>
       </c>
-      <c r="S22">
+      <c r="S22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T22" s="3">
+        <v>9</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="W22" s="3">
+        <v>6</v>
+      </c>
+      <c r="X22" s="3">
         <v>4</v>
       </c>
-      <c r="T22">
-        <v>9</v>
-      </c>
-      <c r="U22">
-        <v>1</v>
-      </c>
-      <c r="V22">
-        <v>10</v>
-      </c>
-      <c r="W22">
-        <v>6</v>
-      </c>
-      <c r="X22">
-        <v>4</v>
-      </c>
-      <c r="Y22">
+      <c r="Y22" s="3">
         <v>139</v>
       </c>
-      <c r="Z22">
+      <c r="Z22" s="4">
         <f>AVERAGE($Y$2:Y22)</f>
         <v>146.52380952380952</v>
       </c>
       <c r="AA22">
-        <f>COUNTIF(D22:X22,10)</f>
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
         <v>2</v>
       </c>
+      <c r="AB22">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>3</v>
+      </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>A22+1</f>
+        <f t="shared" si="15"/>
         <v>22</v>
       </c>
       <c r="B23" s="2">
@@ -4409,81 +4940,86 @@
       <c r="C23">
         <v>7</v>
       </c>
-      <c r="D23">
-        <v>7</v>
-      </c>
-      <c r="E23">
+      <c r="D23" s="3">
+        <v>7</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="3">
+        <v>6</v>
+      </c>
+      <c r="G23" s="3">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3">
+        <v>1</v>
+      </c>
+      <c r="I23" s="3">
+        <v>7</v>
+      </c>
+      <c r="J23" s="3">
+        <v>9</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L23" s="3">
+        <v>7</v>
+      </c>
+      <c r="M23" s="3">
+        <v>2</v>
+      </c>
+      <c r="N23" s="3">
         <v>3</v>
       </c>
-      <c r="F23">
+      <c r="O23" s="3">
+        <v>2</v>
+      </c>
+      <c r="P23" s="3">
         <v>6</v>
       </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="I23">
-        <v>7</v>
-      </c>
-      <c r="J23">
-        <v>9</v>
-      </c>
-      <c r="K23">
-        <v>1</v>
-      </c>
-      <c r="L23">
-        <v>7</v>
-      </c>
-      <c r="M23">
+      <c r="Q23" s="3">
+        <v>3</v>
+      </c>
+      <c r="R23" s="3">
+        <v>8</v>
+      </c>
+      <c r="S23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T23" s="3">
+        <v>6</v>
+      </c>
+      <c r="U23" s="3">
+        <v>0</v>
+      </c>
+      <c r="V23" s="3">
+        <v>6</v>
+      </c>
+      <c r="W23" s="3">
         <v>2</v>
       </c>
-      <c r="N23">
-        <v>3</v>
-      </c>
-      <c r="O23">
-        <v>2</v>
-      </c>
-      <c r="P23">
-        <v>6</v>
-      </c>
-      <c r="Q23">
-        <v>3</v>
-      </c>
-      <c r="R23">
-        <v>8</v>
-      </c>
-      <c r="S23">
-        <v>2</v>
-      </c>
-      <c r="T23">
-        <v>6</v>
-      </c>
-      <c r="U23">
-        <v>0</v>
-      </c>
-      <c r="V23">
-        <v>6</v>
-      </c>
-      <c r="W23">
-        <v>2</v>
-      </c>
-      <c r="Y23">
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3">
         <v>101</v>
       </c>
-      <c r="Z23">
+      <c r="Z23" s="4">
         <f>AVERAGE($Y$2:Y23)</f>
         <v>144.45454545454547</v>
       </c>
       <c r="AA23">
-        <f>COUNTIF(D23:X23,10)</f>
-        <v>0</v>
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
+        <v>0</v>
+      </c>
+      <c r="AB23">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>A23+1</f>
+        <f t="shared" si="15"/>
         <v>23</v>
       </c>
       <c r="B24" s="2">
@@ -4492,70 +5028,667 @@
       <c r="C24">
         <v>7</v>
       </c>
-      <c r="D24">
-        <v>10</v>
-      </c>
-      <c r="F24">
-        <v>9</v>
-      </c>
-      <c r="G24">
+      <c r="D24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3">
+        <v>9</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24" s="3">
+        <v>9</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J24" s="3">
+        <v>8</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L24" s="3">
+        <v>7</v>
+      </c>
+      <c r="M24" s="3">
+        <v>0</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3">
+        <v>9</v>
+      </c>
+      <c r="S24" s="3">
+        <v>0</v>
+      </c>
+      <c r="T24" s="3">
+        <v>5</v>
+      </c>
+      <c r="U24" s="3">
         <v>1</v>
       </c>
-      <c r="H24">
-        <v>9</v>
-      </c>
-      <c r="I24">
-        <v>1</v>
-      </c>
-      <c r="J24">
-        <v>8</v>
-      </c>
-      <c r="K24">
-        <v>2</v>
-      </c>
-      <c r="L24">
-        <v>7</v>
-      </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
-      <c r="N24">
-        <v>10</v>
-      </c>
-      <c r="P24">
-        <v>10</v>
-      </c>
-      <c r="R24">
-        <v>9</v>
-      </c>
-      <c r="S24">
-        <v>0</v>
-      </c>
-      <c r="T24">
-        <v>5</v>
-      </c>
-      <c r="U24">
-        <v>1</v>
-      </c>
-      <c r="V24">
-        <v>9</v>
-      </c>
-      <c r="W24">
-        <v>1</v>
-      </c>
-      <c r="X24">
-        <v>9</v>
-      </c>
-      <c r="Y24">
+      <c r="V24" s="3">
+        <v>9</v>
+      </c>
+      <c r="W24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X24" s="3">
+        <v>9</v>
+      </c>
+      <c r="Y24" s="3">
         <v>163</v>
       </c>
-      <c r="Z24">
+      <c r="Z24" s="4">
         <f>AVERAGE($Y$2:Y24)</f>
         <v>145.2608695652174</v>
       </c>
       <c r="AA24">
-        <f>COUNTIF(D24:X24,10)</f>
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
         <v>3</v>
+      </c>
+      <c r="AB24">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f>A24+1</f>
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>42994</v>
+      </c>
+      <c r="C25">
+        <v>7</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3">
+        <v>8</v>
+      </c>
+      <c r="I25" s="3">
+        <v>1</v>
+      </c>
+      <c r="J25" s="3">
+        <v>7</v>
+      </c>
+      <c r="K25" s="3">
+        <v>0</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3">
+        <v>7</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P25" s="3">
+        <v>9</v>
+      </c>
+      <c r="Q25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R25" s="3">
+        <v>9</v>
+      </c>
+      <c r="S25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T25" s="3">
+        <v>9</v>
+      </c>
+      <c r="U25" s="3">
+        <v>0</v>
+      </c>
+      <c r="V25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="W25" s="3">
+        <v>7</v>
+      </c>
+      <c r="X25" s="3">
+        <v>2</v>
+      </c>
+      <c r="Y25" s="3">
+        <v>160</v>
+      </c>
+      <c r="Z25" s="4">
+        <f>AVERAGE($Y$2:Y25)</f>
+        <v>145.875</v>
+      </c>
+      <c r="AA25">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
+        <v>3</v>
+      </c>
+      <c r="AB25">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f>A25+1</f>
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>42994</v>
+      </c>
+      <c r="C26">
+        <v>7</v>
+      </c>
+      <c r="D26" s="3">
+        <v>7</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="3">
+        <v>4</v>
+      </c>
+      <c r="G26" s="3">
+        <v>4</v>
+      </c>
+      <c r="H26" s="3">
+        <v>8</v>
+      </c>
+      <c r="I26" s="3">
+        <v>0</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3">
+        <v>6</v>
+      </c>
+      <c r="M26" s="3">
+        <v>0</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3">
+        <v>8</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>2</v>
+      </c>
+      <c r="R26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3">
+        <v>3</v>
+      </c>
+      <c r="U26" s="3">
+        <v>4</v>
+      </c>
+      <c r="V26" s="3">
+        <v>8</v>
+      </c>
+      <c r="W26" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X26" s="3">
+        <v>8</v>
+      </c>
+      <c r="Y26" s="3">
+        <v>134</v>
+      </c>
+      <c r="Z26" s="4">
+        <f>AVERAGE($Y$2:Y26)</f>
+        <v>145.4</v>
+      </c>
+      <c r="AA26">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
+        <v>3</v>
+      </c>
+      <c r="AB26">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f>A26+1</f>
+        <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>42994</v>
+      </c>
+      <c r="C27">
+        <v>7</v>
+      </c>
+      <c r="D27" s="3">
+        <v>7</v>
+      </c>
+      <c r="E27" s="3">
+        <v>2</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3">
+        <v>9</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J27" s="3">
+        <v>3</v>
+      </c>
+      <c r="K27" s="3">
+        <v>5</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3">
+        <v>8</v>
+      </c>
+      <c r="O27" s="3">
+        <v>0</v>
+      </c>
+      <c r="P27" s="3">
+        <v>7</v>
+      </c>
+      <c r="Q27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R27" s="3">
+        <v>9</v>
+      </c>
+      <c r="S27" s="3">
+        <v>0</v>
+      </c>
+      <c r="T27" s="3">
+        <v>0</v>
+      </c>
+      <c r="U27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="W27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="X27" s="3">
+        <v>7</v>
+      </c>
+      <c r="Y27" s="3">
+        <v>151</v>
+      </c>
+      <c r="Z27" s="4">
+        <f>AVERAGE($Y$2:Y27)</f>
+        <v>145.61538461538461</v>
+      </c>
+      <c r="AA27">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
+        <v>4</v>
+      </c>
+      <c r="AB27">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f>A27+1</f>
+        <v>27</v>
+      </c>
+      <c r="B28" s="2">
+        <v>42995</v>
+      </c>
+      <c r="C28">
+        <v>11</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3">
+        <v>7</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J28" s="3">
+        <v>6</v>
+      </c>
+      <c r="K28" s="3">
+        <v>0</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3">
+        <v>8</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>1</v>
+      </c>
+      <c r="R28" s="3">
+        <v>9</v>
+      </c>
+      <c r="S28" s="3">
+        <v>0</v>
+      </c>
+      <c r="T28" s="3">
+        <v>8</v>
+      </c>
+      <c r="U28" s="3">
+        <v>0</v>
+      </c>
+      <c r="V28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="W28" s="3">
+        <v>0</v>
+      </c>
+      <c r="X28" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y28" s="3">
+        <v>162</v>
+      </c>
+      <c r="Z28" s="4">
+        <f>AVERAGE($Y$2:Y28)</f>
+        <v>146.22222222222223</v>
+      </c>
+      <c r="AA28">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
+        <v>5</v>
+      </c>
+      <c r="AB28" s="5">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" ref="A29:A31" si="16">A28+1</f>
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>42995</v>
+      </c>
+      <c r="C29">
+        <v>11</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3">
+        <v>9</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3">
+        <v>9</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L29" s="3">
+        <v>8</v>
+      </c>
+      <c r="M29" s="3">
+        <v>1</v>
+      </c>
+      <c r="N29" s="3">
+        <v>5</v>
+      </c>
+      <c r="O29" s="3">
+        <v>4</v>
+      </c>
+      <c r="P29" s="3">
+        <v>9</v>
+      </c>
+      <c r="Q29" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R29" s="3">
+        <v>8</v>
+      </c>
+      <c r="S29" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3">
+        <v>7</v>
+      </c>
+      <c r="W29" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X29" s="3">
+        <v>9</v>
+      </c>
+      <c r="Y29" s="3">
+        <v>173</v>
+      </c>
+      <c r="Z29" s="4">
+        <f>AVERAGE($Y$2:Y29)</f>
+        <v>147.17857142857142</v>
+      </c>
+      <c r="AA29">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
+        <v>3</v>
+      </c>
+      <c r="AB29" s="5">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="16"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="2">
+        <v>42995</v>
+      </c>
+      <c r="C30">
+        <v>11</v>
+      </c>
+      <c r="D30" s="3">
+        <v>7</v>
+      </c>
+      <c r="E30" s="3">
+        <v>1</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3">
+        <v>8</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J30" s="3">
+        <v>8</v>
+      </c>
+      <c r="K30" s="3">
+        <v>0</v>
+      </c>
+      <c r="L30" s="3">
+        <v>1</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N30" s="3">
+        <v>9</v>
+      </c>
+      <c r="O30" s="3">
+        <v>0</v>
+      </c>
+      <c r="P30" s="3">
+        <v>7</v>
+      </c>
+      <c r="Q30" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R30" s="3">
+        <v>4</v>
+      </c>
+      <c r="S30" s="3">
+        <v>4</v>
+      </c>
+      <c r="T30" s="3">
+        <v>3</v>
+      </c>
+      <c r="U30" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V30" s="3">
+        <v>4</v>
+      </c>
+      <c r="W30" s="3">
+        <v>4</v>
+      </c>
+      <c r="X30" s="3"/>
+      <c r="Y30" s="3">
+        <v>126</v>
+      </c>
+      <c r="Z30" s="4">
+        <f>AVERAGE($Y$2:Y30)</f>
+        <v>146.44827586206895</v>
+      </c>
+      <c r="AA30">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
+        <v>1</v>
+      </c>
+      <c r="AB30" s="5">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="16"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="2">
+        <v>42995</v>
+      </c>
+      <c r="C31">
+        <v>11</v>
+      </c>
+      <c r="D31" s="3">
+        <v>9</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3">
+        <v>4</v>
+      </c>
+      <c r="I31" s="3">
+        <v>3</v>
+      </c>
+      <c r="J31" s="3">
+        <v>6</v>
+      </c>
+      <c r="K31" s="3">
+        <v>3</v>
+      </c>
+      <c r="L31" s="3">
+        <v>4</v>
+      </c>
+      <c r="M31" s="3">
+        <v>4</v>
+      </c>
+      <c r="N31" s="3">
+        <v>9</v>
+      </c>
+      <c r="O31" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P31" s="3">
+        <v>8</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>1</v>
+      </c>
+      <c r="R31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U31" s="3"/>
+      <c r="V31" s="3">
+        <v>6</v>
+      </c>
+      <c r="W31" s="3">
+        <v>0</v>
+      </c>
+      <c r="X31" s="3"/>
+      <c r="Y31" s="3">
+        <v>136</v>
+      </c>
+      <c r="Z31" s="4">
+        <f>AVERAGE($Y$2:Y31)</f>
+        <v>146.1</v>
+      </c>
+      <c r="AA31">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=x")</f>
+        <v>3</v>
+      </c>
+      <c r="AB31" s="5">
+        <f>COUNTIF(Table1[[#This Row],[1.1]:[10.3]],"=/")</f>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>